<commit_message>
fix plot dimensions on page 2
</commit_message>
<xml_diff>
--- a/docs/table_template.xlsx
+++ b/docs/table_template.xlsx
@@ -93,16 +93,16 @@
     <t xml:space="preserve">Longfin squid seasonal distribution and growth rates are likely temperature dependent, avoiding water &lt;8°C. Inshore temperature thresholds (around 14°C) initiate migration of squid from offshore overwintering habitats. </t>
   </si>
   <si>
-    <t>com_landings.png</t>
-  </si>
-  <si>
-    <t>com_vessels.png</t>
-  </si>
-  <si>
-    <t>com_revenue.png</t>
-  </si>
-  <si>
-    <t>western_gsi.png</t>
+    <t>Commercial_LONGFINSQUID_Landings_LBS_2025-04-07.png</t>
+  </si>
+  <si>
+    <t>N_Commercial_Vessels_Landing_LONGFINSQUID_2025-04-07.png</t>
+  </si>
+  <si>
+    <t>TOTALANNUALREV_LONGFINSQUID_2023Dols_2025-04-07.png</t>
+  </si>
+  <si>
+    <t>western gulf stream index_2025-04-07.png</t>
   </si>
 </sst>
 </file>
@@ -507,7 +507,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -552,7 +552,7 @@
         <v>19</v>
       </c>
       <c r="E2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -572,7 +572,7 @@
         <v>20</v>
       </c>
       <c r="E3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -592,7 +592,7 @@
         <v>21</v>
       </c>
       <c r="E4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -612,7 +612,7 @@
         <v>22</v>
       </c>
       <c r="E5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -632,7 +632,7 @@
         <v>7</v>
       </c>
       <c r="E6">
-        <v>2.33</v>
+        <v>3</v>
       </c>
       <c r="F6">
         <v>1</v>

</xml_diff>

<commit_message>
add bottom temp indicator
</commit_message>
<xml_diff>
--- a/docs/table_template.xlsx
+++ b/docs/table_template.xlsx
@@ -56,12 +56,6 @@
     <t>Add implications here (3-5 sentences)</t>
   </si>
   <si>
-    <t>noaa_logo.png</t>
-  </si>
-  <si>
-    <t>Add status in 2024 here (short phrase)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Commercial landings (millions of lbs.)
 </t>
   </si>
@@ -75,9 +69,6 @@
     <t>Commercial revenue (2023 USD)</t>
   </si>
   <si>
-    <t>Bottom temperature (°C)</t>
-  </si>
-  <si>
     <t>Above long term average</t>
   </si>
   <si>
@@ -90,19 +81,28 @@
     <t>Since the mid-1990s, north and westward shifts in the Gulf Stream have resulted in an increase in warm core rings and deep water, high salinity heat waves. The position of the Gulf Stream influences seasonal temperature and water mass mixing dynamics that affect longfin squid habitat suitability, temperature-dependent growth, and prey availability.</t>
   </si>
   <si>
+    <t>Commercial_LONGFINSQUID_Landings_LBS_2025-04-07.png</t>
+  </si>
+  <si>
+    <t>N_Commercial_Vessels_Landing_LONGFINSQUID_2025-04-07.png</t>
+  </si>
+  <si>
+    <t>TOTALANNUALREV_LONGFINSQUID_2023Dols_2025-04-07.png</t>
+  </si>
+  <si>
+    <t>western gulf stream index_2025-04-07.png</t>
+  </si>
+  <si>
+    <t>Above long term average (Fall); near long term average (Spring)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bottom temperature in MAB and SNE(°C) </t>
+  </si>
+  <si>
+    <t>BottomT_2025-04-10.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">Longfin squid seasonal distribution and growth rates are likely temperature dependent, avoiding water &lt;8°C. Inshore temperature thresholds (around 14°C) initiate migration of squid from offshore overwintering habitats. </t>
-  </si>
-  <si>
-    <t>Commercial_LONGFINSQUID_Landings_LBS_2025-04-07.png</t>
-  </si>
-  <si>
-    <t>N_Commercial_Vessels_Landing_LONGFINSQUID_2025-04-07.png</t>
-  </si>
-  <si>
-    <t>TOTALANNUALREV_LONGFINSQUID_2023Dols_2025-04-07.png</t>
-  </si>
-  <si>
-    <t>western gulf stream index_2025-04-07.png</t>
   </si>
 </sst>
 </file>
@@ -507,7 +507,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -540,16 +540,16 @@
     </row>
     <row r="2" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E2">
         <v>3</v>
@@ -560,16 +560,16 @@
     </row>
     <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E3">
         <v>3</v>
@@ -580,16 +580,16 @@
     </row>
     <row r="4" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -600,16 +600,16 @@
     </row>
     <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -620,22 +620,22 @@
     </row>
     <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="E6">
         <v>3</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update bt axes and plot
</commit_message>
<xml_diff>
--- a/docs/table_template.xlsx
+++ b/docs/table_template.xlsx
@@ -99,10 +99,10 @@
     <t xml:space="preserve">Bottom temperature in MAB and SNE(°C) </t>
   </si>
   <si>
-    <t>BottomT_2025-04-10.png</t>
-  </si>
-  <si>
     <t xml:space="preserve">Longfin squid seasonal distribution and growth rates are likely temperature dependent, avoiding water &lt;8°C. Inshore temperature thresholds (around 14°C) initiate migration of squid from offshore overwintering habitats. </t>
+  </si>
+  <si>
+    <t>BottomT_2025-04-17.png</t>
   </si>
 </sst>
 </file>
@@ -507,7 +507,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -626,10 +626,10 @@
         <v>19</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
         <v>22</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
       </c>
       <c r="E6">
         <v>3</v>

</xml_diff>

<commit_message>
change font in flextable
</commit_message>
<xml_diff>
--- a/docs/table_template.xlsx
+++ b/docs/table_template.xlsx
@@ -50,9 +50,6 @@
     <t>w</t>
   </si>
   <si>
-    <t>h</t>
-  </si>
-  <si>
     <t>Add implications here (3-5 sentences)</t>
   </si>
   <si>
@@ -103,6 +100,9 @@
   </si>
   <si>
     <t>BottomT_2025-04-17.png</t>
+  </si>
+  <si>
+    <t>h</t>
   </si>
 </sst>
 </file>
@@ -507,7 +507,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -535,21 +535,21 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2">
         <v>3</v>
@@ -560,16 +560,16 @@
     </row>
     <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3">
         <v>3</v>
@@ -580,16 +580,16 @@
     </row>
     <row r="4" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -600,16 +600,16 @@
     </row>
     <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -620,16 +620,16 @@
     </row>
     <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" t="s">
         <v>21</v>
-      </c>
-      <c r="D6" t="s">
-        <v>22</v>
       </c>
       <c r="E6">
         <v>3</v>

</xml_diff>

<commit_message>
some text edits and fix title
</commit_message>
<xml_diff>
--- a/docs/table_template.xlsx
+++ b/docs/table_template.xlsx
@@ -63,9 +63,6 @@
     <t>Western Gulf Stream Index (shift in the western part of the Gulf Stream North wall: mean position: &gt;0 = more northerly, &lt;0 = more southerly)</t>
   </si>
   <si>
-    <t>Commercial revenue (2023 USD)</t>
-  </si>
-  <si>
     <t>Above long term average</t>
   </si>
   <si>
@@ -103,6 +100,9 @@
   </si>
   <si>
     <t>h</t>
+  </si>
+  <si>
+    <t>Commercial revenue (millions of 2023 USD)</t>
   </si>
 </sst>
 </file>
@@ -507,7 +507,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -535,7 +535,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -543,13 +543,13 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2">
         <v>3</v>
@@ -563,13 +563,13 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3">
         <v>3</v>
@@ -580,16 +580,16 @@
     </row>
     <row r="4" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -603,13 +603,13 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -620,16 +620,16 @@
     </row>
     <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" t="s">
         <v>20</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
       </c>
       <c r="E6">
         <v>3</v>

</xml_diff>

<commit_message>
run report card with 2024 commercial data
</commit_message>
<xml_diff>
--- a/docs/table_template.xlsx
+++ b/docs/table_template.xlsx
@@ -75,15 +75,6 @@
     <t>Since the mid-1990s, north and westward shifts in the Gulf Stream have resulted in an increase in warm core rings and deep water, high salinity heat waves. The position of the Gulf Stream influences seasonal temperature and water mass mixing dynamics that affect longfin squid habitat suitability, temperature-dependent growth, and prey availability.</t>
   </si>
   <si>
-    <t>Commercial_LONGFINSQUID_Landings_LBS_2025-04-07.png</t>
-  </si>
-  <si>
-    <t>N_Commercial_Vessels_Landing_LONGFINSQUID_2025-04-07.png</t>
-  </si>
-  <si>
-    <t>TOTALANNUALREV_LONGFINSQUID_2023Dols_2025-04-07.png</t>
-  </si>
-  <si>
     <t>western gulf stream index_2025-04-07.png</t>
   </si>
   <si>
@@ -103,6 +94,15 @@
   </si>
   <si>
     <t>Commercial revenue (millions of 2023 USD)</t>
+  </si>
+  <si>
+    <t>Commercial_LONGFINSQUID_Landings_LBS_2025-05-05.png</t>
+  </si>
+  <si>
+    <t>N_Commercial_Vessels_Landing_LONGFINSQUID_2025-05-05.png</t>
+  </si>
+  <si>
+    <t>TOTALANNUALREV_LONGFINSQUID_2024Dols_2025-05-05.png</t>
   </si>
 </sst>
 </file>
@@ -507,7 +507,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -535,7 +535,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -549,7 +549,7 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E2">
         <v>3</v>
@@ -569,7 +569,7 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E3">
         <v>3</v>
@@ -580,7 +580,7 @@
     </row>
     <row r="4" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -589,7 +589,7 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -609,7 +609,7 @@
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -620,16 +620,16 @@
     </row>
     <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
         <v>17</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" t="s">
-        <v>20</v>
       </c>
       <c r="E6">
         <v>3</v>

</xml_diff>

<commit_message>
add edits to report card doc
</commit_message>
<xml_diff>
--- a/docs/table_template.xlsx
+++ b/docs/table_template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stephanie.owen\Documents\longfinESP\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\nefscdata\SOE_ESP_Data\longfinESP\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74383B57-F681-4154-BCF7-CD277B501C86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26556" yWindow="-2712" windowWidth="21600" windowHeight="11232"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Indicator (units)</t>
   </si>
@@ -51,9 +43,6 @@
   </si>
   <si>
     <t>h</t>
-  </si>
-  <si>
-    <t>Add implications here (3-5 sentences)</t>
   </si>
   <si>
     <t xml:space="preserve">Commercial landings (millions of lbs.)
@@ -66,9 +55,6 @@
     <t>Western Gulf Stream Index (shift in the western part of the Gulf Stream North wall: mean position: &gt;0 = more northerly, &lt;0 = more southerly)</t>
   </si>
   <si>
-    <t>Commercial revenue (2023 USD)</t>
-  </si>
-  <si>
     <t>Above long term average</t>
   </si>
   <si>
@@ -103,12 +89,24 @@
   </si>
   <si>
     <t>BottomT_2025-04-17.png</t>
+  </si>
+  <si>
+    <t>Commercial revenue (2024 USD)</t>
+  </si>
+  <si>
+    <t>Number of commercial vessels has been steadily decreasing since around 2000 consistent with decreasing fleet diversity and continued risk to fishery resilience (MAFMC FID).</t>
+  </si>
+  <si>
+    <t>Average Longfin ex-vessel prices in 2024 increased slightly from 2023 (+10%), but commercial revenue has decreased from 2023 which is most likely driven by a an overall decrease in landings by 23% (MAFMC FID).</t>
+  </si>
+  <si>
+    <t>An increase in landings since 2020 but decrease in number of vessels could indicate targeted trips in specific times of year and fishers targeting other species when longfin are not available. High variability in landings is common for squid fisheries, and 2024 commercial landings fall within the long term mean.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -503,11 +501,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -540,16 +538,16 @@
     </row>
     <row r="2" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E2">
         <v>3</v>
@@ -560,16 +558,16 @@
     </row>
     <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E3">
         <v>3</v>
@@ -580,16 +578,16 @@
     </row>
     <row r="4" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -600,16 +598,16 @@
     </row>
     <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
       <c r="C5" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -620,16 +618,16 @@
     </row>
     <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
         <v>20</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" t="s">
-        <v>22</v>
       </c>
       <c r="E6">
         <v>3</v>

</xml_diff>

<commit_message>
update table template with most recent commercial plots
</commit_message>
<xml_diff>
--- a/docs/table_template.xlsx
+++ b/docs/table_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\nefscdata\SOE_ESP_Data\longfinESP\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74383B57-F681-4154-BCF7-CD277B501C86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE8D4CD-FA51-43CF-BEDC-4EFCC89F8FB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -67,15 +67,6 @@
     <t>Since the mid-1990s, north and westward shifts in the Gulf Stream have resulted in an increase in warm core rings and deep water, high salinity heat waves. The position of the Gulf Stream influences seasonal temperature and water mass mixing dynamics that affect longfin squid habitat suitability, temperature-dependent growth, and prey availability.</t>
   </si>
   <si>
-    <t>Commercial_LONGFINSQUID_Landings_LBS_2025-04-07.png</t>
-  </si>
-  <si>
-    <t>N_Commercial_Vessels_Landing_LONGFINSQUID_2025-04-07.png</t>
-  </si>
-  <si>
-    <t>TOTALANNUALREV_LONGFINSQUID_2023Dols_2025-04-07.png</t>
-  </si>
-  <si>
     <t>western gulf stream index_2025-04-07.png</t>
   </si>
   <si>
@@ -101,6 +92,15 @@
   </si>
   <si>
     <t>An increase in landings since 2020 but decrease in number of vessels could indicate targeted trips in specific times of year and fishers targeting other species when longfin are not available. High variability in landings is common for squid fisheries, and 2024 commercial landings fall within the long term mean.</t>
+  </si>
+  <si>
+    <t>Commercial_LONGFINSQUID_Landings_LBS_2025-05-05.png</t>
+  </si>
+  <si>
+    <t>N_Commercial_Vessels_Landing_LONGFINSQUID_2025-05-05.png</t>
+  </si>
+  <si>
+    <t>TOTALANNUALREV_LONGFINSQUID_2023Dols_2025-05-05.png</t>
   </si>
 </sst>
 </file>
@@ -505,7 +505,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -544,10 +544,10 @@
         <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="E2">
         <v>3</v>
@@ -564,10 +564,10 @@
         <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="E3">
         <v>3</v>
@@ -578,16 +578,16 @@
     </row>
     <row r="4" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -607,7 +607,7 @@
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -618,16 +618,16 @@
     </row>
     <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
         <v>17</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" t="s">
-        <v>20</v>
       </c>
       <c r="E6">
         <v>3</v>

</xml_diff>

<commit_message>
update gsi indicator and plot
</commit_message>
<xml_diff>
--- a/docs/table_template.xlsx
+++ b/docs/table_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\nefscdata\SOE_ESP_Data\longfinESP\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE8D4CD-FA51-43CF-BEDC-4EFCC89F8FB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0C1AE03-10A8-4709-9FAE-D60D86AE2C16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -67,9 +67,6 @@
     <t>Since the mid-1990s, north and westward shifts in the Gulf Stream have resulted in an increase in warm core rings and deep water, high salinity heat waves. The position of the Gulf Stream influences seasonal temperature and water mass mixing dynamics that affect longfin squid habitat suitability, temperature-dependent growth, and prey availability.</t>
   </si>
   <si>
-    <t>western gulf stream index_2025-04-07.png</t>
-  </si>
-  <si>
     <t>Above long term average (Fall); near long term average (Spring)</t>
   </si>
   <si>
@@ -101,6 +98,9 @@
   </si>
   <si>
     <t>TOTALANNUALREV_LONGFINSQUID_2023Dols_2025-05-05.png</t>
+  </si>
+  <si>
+    <t>western gulf stream index_2025-05-29.png</t>
   </si>
 </sst>
 </file>
@@ -505,7 +505,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -544,10 +544,10 @@
         <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
         <v>21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>22</v>
       </c>
       <c r="E2">
         <v>3</v>
@@ -564,10 +564,10 @@
         <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3">
         <v>3</v>
@@ -578,16 +578,16 @@
     </row>
     <row r="4" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -607,7 +607,7 @@
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -618,16 +618,16 @@
     </row>
     <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" t="s">
         <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
       </c>
       <c r="E6">
         <v>3</v>

</xml_diff>

<commit_message>
update report card doc and table template with squid squad suggestions
</commit_message>
<xml_diff>
--- a/docs/table_template.xlsx
+++ b/docs/table_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abigail.tyrell\Documents\code\longfinESP\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\nefscdata\SOE_ESP_Data\longfinESP\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{174BDCEA-C9EE-49E5-BA13-3CDF90D02386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19BD0DD3-3712-419B-B103-464F3AA38311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28320" yWindow="-6525" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -49,9 +49,6 @@
 </t>
   </si>
   <si>
-    <t>Number of commercial vessels (#)</t>
-  </si>
-  <si>
     <t>Western Gulf Stream Index (shift in the western part of the Gulf Stream North wall: mean position: &gt;0 = more northerly, &lt;0 = more southerly)</t>
   </si>
   <si>
@@ -73,24 +70,15 @@
     <t xml:space="preserve">Bottom temperature in MAB and SNE(°C) </t>
   </si>
   <si>
-    <t xml:space="preserve">Longfin squid seasonal distribution and growth rates are likely temperature dependent, avoiding water &lt;8°C. Inshore temperature thresholds (around 14°C) initiate migration of squid from offshore overwintering habitats. </t>
-  </si>
-  <si>
     <t>BottomT_2025-04-17.png</t>
   </si>
   <si>
     <t>Commercial revenue (2024 USD)</t>
   </si>
   <si>
-    <t>Number of commercial vessels has been steadily decreasing since around 2000 consistent with decreasing fleet diversity and continued risk to fishery resilience (MAFMC FID).</t>
-  </si>
-  <si>
     <t>Average Longfin ex-vessel prices in 2024 increased slightly from 2023 (+10%), but commercial revenue has decreased from 2023 which is most likely driven by a an overall decrease in landings by 23% (MAFMC FID).</t>
   </si>
   <si>
-    <t>An increase in landings since 2020 but decrease in number of vessels could indicate targeted trips in specific times of year and fishers targeting other species when longfin are not available. High variability in landings is common for squid fisheries, and 2024 commercial landings fall within the long term mean.</t>
-  </si>
-  <si>
     <t>Commercial_LONGFINSQUID_Landings_LBS_2025-05-05.png</t>
   </si>
   <si>
@@ -101,6 +89,18 @@
   </si>
   <si>
     <t>TOTALANNUALREV_LONGFINSQUID_2024Dols_2025-05-05.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Environmental dynamics vary between locations/timing of the summer and winter squid fisheries. An increase in landings since 2020 but decrease in number of vessels could indicate targeted trips in specific times of year and fishers targeting other species when longfin are not available. </t>
+  </si>
+  <si>
+    <t>Number of commercial vessels (#  of federally-permitted vessels landing over 1lb of longfin squid)</t>
+  </si>
+  <si>
+    <t>Number of commercial vessels has been steadily decreasing since around 2000 consistent with decreasing fleet diversity and continued risk to fishery resilience (MAFMC FID). Permit requalification in 2019 and a decrease in the incidental limit for trimester 2 resulted in fishery closures in 2022 and 2023, which may contribute to decreased participation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inshore temperature thresholds (around 14°C) initiate migration of squid from offshore overwintering habitats. Longfin squid seasonal distribution and growth rates are likely temperature dependent, avoiding water &lt;8°C. 2024 spring bottom temperatures are near the long term mean, however cold pool temperatures dipped below 8°C. </t>
   </si>
 </sst>
 </file>
@@ -505,7 +505,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -541,13 +541,13 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E2">
         <v>3</v>
@@ -558,16 +558,16 @@
     </row>
     <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
         <v>18</v>
-      </c>
-      <c r="D3" t="s">
-        <v>22</v>
       </c>
       <c r="E3">
         <v>3</v>
@@ -578,16 +578,16 @@
     </row>
     <row r="4" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -598,16 +598,16 @@
     </row>
     <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
       <c r="C5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -618,16 +618,16 @@
     </row>
     <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
         <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
       </c>
       <c r="E6">
         <v>3</v>

</xml_diff>

<commit_message>
risk and table text edits
</commit_message>
<xml_diff>
--- a/docs/table_template.xlsx
+++ b/docs/table_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\nefscdata\SOE_ESP_Data\longfinESP\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stephanie.owen\Documents\longfinESP\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19BD0DD3-3712-419B-B103-464F3AA38311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D111CF6C-0038-43F7-ADD2-02ECBB6C7C42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,9 +61,6 @@
     <t>Near long term average</t>
   </si>
   <si>
-    <t>Since the mid-1990s, north and westward shifts in the Gulf Stream have resulted in an increase in warm core rings and deep water, high salinity heat waves. The position of the Gulf Stream influences seasonal temperature and water mass mixing dynamics that affect longfin squid habitat suitability, temperature-dependent growth, and prey availability.</t>
-  </si>
-  <si>
     <t>Above long term average (Fall); near long term average (Spring)</t>
   </si>
   <si>
@@ -73,9 +70,6 @@
     <t>BottomT_2025-04-17.png</t>
   </si>
   <si>
-    <t>Commercial revenue (2024 USD)</t>
-  </si>
-  <si>
     <t>Average Longfin ex-vessel prices in 2024 increased slightly from 2023 (+10%), but commercial revenue has decreased from 2023 which is most likely driven by a an overall decrease in landings by 23% (MAFMC FID).</t>
   </si>
   <si>
@@ -100,7 +94,13 @@
     <t>Number of commercial vessels has been steadily decreasing since around 2000 consistent with decreasing fleet diversity and continued risk to fishery resilience (MAFMC FID). Permit requalification in 2019 and a decrease in the incidental limit for trimester 2 resulted in fishery closures in 2022 and 2023, which may contribute to decreased participation.</t>
   </si>
   <si>
-    <t xml:space="preserve">Inshore temperature thresholds (around 14°C) initiate migration of squid from offshore overwintering habitats. Longfin squid seasonal distribution and growth rates are likely temperature dependent, avoiding water &lt;8°C. 2024 spring bottom temperatures are near the long term mean, however cold pool temperatures dipped below 8°C. </t>
+    <t>Commercial revenue (millions 2024 USD)</t>
+  </si>
+  <si>
+    <t>Inshore temperature thresholds (around 14°C) initiate migration of squid from offshore overwintering habitats. Longfin squid seasonal distribution and growth rates are likely temperature dependent, avoiding water &lt;8°C. Stronger and/or more persistent Mid-Atlantic Cold Pool conditions (not shown) may limit habitat availability (https://noaa-edab.github.io/catalog/cold_pool.html).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Since the mid-1990s, north and westward shifts in the Gulf Stream have resulted in an increase in warm core rings and deep water, high salinity heat waves. The position of the Gulf Stream influences seasonal temperature and water mass mixing dynamics that affect longfin squid habitat suitability, temperature-dependent growth, and prey availability (https://noaa-edab.github.io/catalog/gsi.html). </t>
   </si>
 </sst>
 </file>
@@ -505,7 +505,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -544,10 +544,10 @@
         <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E2">
         <v>3</v>
@@ -558,16 +558,16 @@
     </row>
     <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E3">
         <v>3</v>
@@ -578,16 +578,16 @@
     </row>
     <row r="4" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -604,10 +604,10 @@
         <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -618,16 +618,16 @@
     </row>
     <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
         <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
       </c>
       <c r="E6">
         <v>3</v>

</xml_diff>

<commit_message>
update gsi indicator for 2025
</commit_message>
<xml_diff>
--- a/docs/table_template.xlsx
+++ b/docs/table_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stephanie.owen\Documents\longfinESP\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B01FDA33-25F0-400E-B1C3-CC9B1A41111D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4FAF310-4AA8-4129-8476-A40DC1DE0888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36" yWindow="72" windowWidth="11232" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,9 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
@@ -64,9 +67,6 @@
     <t>N_Commercial_Vessels_Landing_LONGFINSQUID_2025-05-05.png</t>
   </si>
   <si>
-    <t>western gulf stream index_2025-05-29.png</t>
-  </si>
-  <si>
     <t>TOTALANNUALREV_LONGFINSQUID_2024Dols_2025-05-05.png</t>
   </si>
   <si>
@@ -97,9 +97,6 @@
 decrease in landings by 23% [7].</t>
   </si>
   <si>
-    <t>Above long term (1996-2024) average</t>
-  </si>
-  <si>
     <t>Above long term (1996-2024) average (Fall); near long term (1996-2024) average (Spring)</t>
   </si>
   <si>
@@ -107,6 +104,12 @@
 decreasing since around 2000 consistent with
 decreasing fleet diversity and continued risk to
 fishery resilience [7]. Permit requalification in 2019 and a decrease in the post-closure trip  limit for trimester 2 may cap participation, although these actions were designed to accommodate recent fishing trends and activity. </t>
+  </si>
+  <si>
+    <t>Near long term (1996-2025) average</t>
+  </si>
+  <si>
+    <t>western gulf stream index_2026-02-23.png</t>
   </si>
 </sst>
 </file>
@@ -514,7 +517,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -550,10 +553,10 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -567,13 +570,13 @@
     </row>
     <row r="3" spans="1:6" ht="172.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
@@ -587,16 +590,16 @@
     </row>
     <row r="4" spans="1:6" ht="93" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -610,13 +613,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -630,10 +633,10 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
rerun snapshot with 2025 commercial indicators
</commit_message>
<xml_diff>
--- a/docs/table_template.xlsx
+++ b/docs/table_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stephanie.owen\Documents\longfinESP\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4FAF310-4AA8-4129-8476-A40DC1DE0888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07CB7612-1A22-455A-BB06-14A2A5EE9D11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>Indicator (units)</t>
   </si>
@@ -61,15 +61,6 @@
     <t>BottomT_2025-04-17.png</t>
   </si>
   <si>
-    <t>Commercial_LONGFINSQUID_Landings_LBS_2025-05-05.png</t>
-  </si>
-  <si>
-    <t>N_Commercial_Vessels_Landing_LONGFINSQUID_2025-05-05.png</t>
-  </si>
-  <si>
-    <t>TOTALANNUALREV_LONGFINSQUID_2024Dols_2025-05-05.png</t>
-  </si>
-  <si>
     <t xml:space="preserve">Environmental dynamics vary between locations/timing of the summer and winter squid fisheries. An increase in landings since 2020 but decrease in number of vessels could indicate targeted trips in specific times of year and fishers targeting other species when longfin are not available. </t>
   </si>
   <si>
@@ -82,34 +73,38 @@
     <t xml:space="preserve">Since the mid-1990s, north and westward shifts in the Gulf Stream have resulted in an increase in warm core rings and deep water, high salinity heat waves. The position of the Gulf Stream influences seasonal temperature and water mass mixing dynamics that affect longfin squid habitat suitability, temperature-dependent growth, and prey availability (https://noaa-edab.github.io/catalog/gsi.html). </t>
   </si>
   <si>
-    <t>Near long term (1996-2024) average</t>
-  </si>
-  <si>
-    <t>Below long term (1996-2024) average</t>
-  </si>
-  <si>
-    <t>Commercial revenue (millions, inflation adjusted to 2024 USD)</t>
-  </si>
-  <si>
-    <t>Average longfin ex-vessel prices in 2024
-increased slightly from 2023 (+10%), but
-commercial revenue has decreased from 2023, driven by the overall
-decrease in landings by 23% [7].</t>
-  </si>
-  <si>
     <t>Above long term (1996-2024) average (Fall); near long term (1996-2024) average (Spring)</t>
   </si>
   <si>
+    <t>Near long term (1996-2025) average</t>
+  </si>
+  <si>
+    <t>western gulf stream index_2026-02-23.png</t>
+  </si>
+  <si>
+    <t>Below long term (1996-2025) average</t>
+  </si>
+  <si>
     <t xml:space="preserve">Number of commercial vessels has been steadily
-decreasing since around 2000 consistent with
+decreasing since around 2000 (although has slightly increased in 2025) consistent with
 decreasing fleet diversity and continued risk to
 fishery resilience [7]. Permit requalification in 2019 and a decrease in the post-closure trip  limit for trimester 2 may cap participation, although these actions were designed to accommodate recent fishing trends and activity. </t>
   </si>
   <si>
-    <t>Near long term (1996-2025) average</t>
-  </si>
-  <si>
-    <t>western gulf stream index_2026-02-23.png</t>
+    <t>Commercial revenue (millions, inflation adjusted to 2025 USD)</t>
+  </si>
+  <si>
+    <t>Average longfin ex-vessel prices in 2024 increased slightly from 2023 (+10%). Commercial revenue has decreased since 2022, driven by the overall
+decrease in landings by 23% [7].</t>
+  </si>
+  <si>
+    <t>Commercial_LONGFINSQUID_Landings_LBS_2026-02-25.png</t>
+  </si>
+  <si>
+    <t>N_Commercial_Vessels_Landing_LONGFINSQUID_2026-02-25.png</t>
+  </si>
+  <si>
+    <t>TOTALANNUALREV_LONGFINSQUID_2025Dols_2026-02-25.png</t>
   </si>
 </sst>
 </file>
@@ -517,7 +512,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -553,13 +548,13 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="E2">
         <v>3</v>
@@ -568,18 +563,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="172.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="185.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" t="s">
         <v>22</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
       </c>
       <c r="E3">
         <v>3</v>
@@ -588,18 +583,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="93" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="79.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -613,13 +608,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
         <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>24</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -633,10 +628,10 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>

</xml_diff>